<commit_message>
Added 1, 1v15, and 3v3 regulators/Updated parts list
</commit_message>
<xml_diff>
--- a/Parts List.xlsx
+++ b/Parts List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexl\Desktop\WiiPowerSupply\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DFE1AAC-49C4-4467-95DF-6B930739CC18}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78D0BE5-4E0E-449A-BEF4-36E27CD015C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6270" yWindow="4170" windowWidth="15375" windowHeight="7965" xr2:uid="{EE5EBFFE-520B-449B-AFB7-7B7C4DFECCED}"/>
+    <workbookView xWindow="28680" yWindow="4365" windowWidth="20730" windowHeight="11160" xr2:uid="{EE5EBFFE-520B-449B-AFB7-7B7C4DFECCED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,28 +31,315 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t xml:space="preserve">MCP6L01RT-E/OT </t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/microchip-technology/MCP6L01RT-E-OT/MCP6L01RT-E-OTCT-ND/2060326</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>IC OPAMP GP 1MHZ RRO SOT23-5</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Customer Reference</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>Backorder</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Extended Price USD</t>
+  </si>
+  <si>
+    <t>NCP3170ADR2GOSCT-ND</t>
+  </si>
+  <si>
+    <t>NCP3170ADR2G</t>
+  </si>
+  <si>
+    <t>IC REG BUCK ADJ 3A SYNC 8SOIC</t>
+  </si>
+  <si>
+    <t>REG_IC</t>
+  </si>
+  <si>
+    <t>311-1141-1-ND</t>
+  </si>
+  <si>
+    <t>CC0805KRX7R8BB104</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 25V X7R 0805</t>
+  </si>
+  <si>
+    <t>REG_INPUT_BYPASS</t>
+  </si>
+  <si>
+    <t>493-2179-1-ND</t>
+  </si>
+  <si>
+    <t>UWT1C221MCL1GS</t>
+  </si>
+  <si>
+    <t>CAP ALUM 220UF 20% 16V SMD</t>
+  </si>
+  <si>
+    <t>REG_INPUT_SMOOTH</t>
+  </si>
+  <si>
+    <t>SRU8043-4R7YCT-ND</t>
+  </si>
+  <si>
+    <t>SRU8043-4R7Y</t>
+  </si>
+  <si>
+    <t>FIXED IND 4.7UH 4.6A 17 MOHM SMD</t>
+  </si>
+  <si>
+    <t>REG_IND</t>
+  </si>
+  <si>
+    <t>490-10530-1-ND</t>
+  </si>
+  <si>
+    <t>GRM32EC70J107ME15L</t>
+  </si>
+  <si>
+    <t>CAP CER 100UF 6.3V X7S 1210</t>
+  </si>
+  <si>
+    <t>REG_OUT_SMOOTH</t>
+  </si>
+  <si>
+    <t>RR12P1.0KDCT-ND</t>
+  </si>
+  <si>
+    <t>RR1220P-102-D</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 0.5% 1/10W 0805</t>
+  </si>
+  <si>
+    <t>REG_RF &amp; REG_R1_1V15</t>
+  </si>
+  <si>
+    <t>311-4304-1-ND</t>
+  </si>
+  <si>
+    <t>CC0805KRX7R0BB183</t>
+  </si>
+  <si>
+    <t>CAP CER 0.018UF 100V X7R 0805</t>
+  </si>
+  <si>
+    <t>REG_CC_LV</t>
+  </si>
+  <si>
+    <t>1276-2533-1-ND</t>
+  </si>
+  <si>
+    <t>CL21B511KBANNNC</t>
+  </si>
+  <si>
+    <t>CAP CER 510PF 50V X7R 0805</t>
+  </si>
+  <si>
+    <t>REG_CP_1V</t>
+  </si>
+  <si>
+    <t>490-12745-1-ND</t>
+  </si>
+  <si>
+    <t>GRM2165C2A162JA01D</t>
+  </si>
+  <si>
+    <t>CAP CER 1600PF 100V C0G/NP0 0805</t>
+  </si>
+  <si>
+    <t>REG_CF_1V</t>
+  </si>
+  <si>
+    <t>311-1.87KCRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0805FR-071K87L</t>
+  </si>
+  <si>
+    <t>RES SMD 1.87K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>REG_R1_1V</t>
+  </si>
+  <si>
+    <t>A126387CT-ND</t>
+  </si>
+  <si>
+    <t>CRG0805F7K5</t>
+  </si>
+  <si>
+    <t>RES SMD 7.5K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>REG_R2_1V</t>
+  </si>
+  <si>
+    <t>311-1.78KCRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0805FR-071K78L</t>
+  </si>
+  <si>
+    <t>RES SMD 1.78K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>REG_RC_1V</t>
+  </si>
+  <si>
+    <t>732-7856-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 470PF 50V C0G/NP0 0805</t>
+  </si>
+  <si>
+    <t>REG_CP_1V15</t>
+  </si>
+  <si>
+    <t>490-8290-1-ND</t>
+  </si>
+  <si>
+    <t>GRM2165C2A132JA01D</t>
+  </si>
+  <si>
+    <t>CAP CER 1300PF 100V C0G/NP0 0805</t>
+  </si>
+  <si>
+    <t>REG_CF_1V15 &amp; 3V3</t>
+  </si>
+  <si>
+    <t>311-2.10KCRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0805FR-072K1L</t>
+  </si>
+  <si>
+    <t>RES SMD 2.1K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>REG_RC_1V15</t>
+  </si>
+  <si>
+    <t>311-2.20KCRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0805FR-072K2L</t>
+  </si>
+  <si>
+    <t>RES SMD 2.2K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>REG_R2_1V15</t>
+  </si>
+  <si>
+    <t>RNCP0805FTD1K50CT-ND</t>
+  </si>
+  <si>
+    <t>RNCP0805FTD1K50</t>
+  </si>
+  <si>
+    <t>RES 1.5K OHM 1% 1/4W 0805</t>
+  </si>
+  <si>
+    <t>REG_R2_3V3</t>
+  </si>
+  <si>
+    <t>311-4.64KCRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0805FR-074K64L</t>
+  </si>
+  <si>
+    <t>RES SMD 4.64K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>REG_R1_3V3</t>
+  </si>
+  <si>
+    <t>478-1384-1-ND</t>
+  </si>
+  <si>
+    <t>08055C123KAT2A</t>
+  </si>
+  <si>
+    <t>CAP CER 0.012UF 50V X7R 0805</t>
+  </si>
+  <si>
+    <t>REG_CC_3V3</t>
+  </si>
+  <si>
+    <t>311-8.45KCRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0805FR-078K45L</t>
+  </si>
+  <si>
+    <t>RES SMD 8.45K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>REG_RC_3V3</t>
+  </si>
+  <si>
+    <t>1276-1836-1-ND</t>
+  </si>
+  <si>
+    <t>CL21C910JBANNNC</t>
+  </si>
+  <si>
+    <t>CAP CER 91PF 50V C0G/NP0 0805</t>
+  </si>
+  <si>
+    <t>REG_CP_3V3</t>
+  </si>
+  <si>
+    <t>MCP6L01RT-E/OTCT-ND</t>
+  </si>
+  <si>
+    <t>MCP6L01RT-E/OT</t>
+  </si>
+  <si>
+    <t>CHARGE_OPAMP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -75,8 +362,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,26 +682,760 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877CC8D1-C29E-4C1B-9BF0-5B110EF9C307}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="J2" s="4">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2">
+        <v>3</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="J4" s="4">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="2">
+        <v>3</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="J5" s="4">
+        <v>2.94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="2">
+        <v>3</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="J6" s="4">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="2">
+        <v>4</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.17</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="2">
+        <v>885012007061</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.17</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0.26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>